<commit_message>
tweaked tables and text
</commit_message>
<xml_diff>
--- a/data/search_records_precip_meta_analysis.xlsx
+++ b/data/search_records_precip_meta_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\work\Projects\In_progress\precip_changes_soil_fauna\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FE557C-3F7F-4A0E-AC0C-25D082ADC0FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E47FE3-3B1A-4570-9E7C-34FCF5BD5C8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8625" activeTab="1" xr2:uid="{05EA8098-D558-4960-9E80-FB1BB65BD2EC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -94,18 +94,12 @@
     <t>Excluded full texts (not in English)</t>
   </si>
   <si>
-    <t>Excluded full texts (no PECO element)</t>
-  </si>
-  <si>
     <t>Articles in the review</t>
   </si>
   <si>
     <t>Studies in the review</t>
   </si>
   <si>
-    <t>Studies included in the map</t>
-  </si>
-  <si>
     <t>TITLE-ABS-KEY((forest* OR woodland* OR plantation* OR clearcut OR logg* OR timber) AND (soil* OR below?ground OR root*) AND (drought* OR *fire* OR burn* OR wind* OR typhoon* OR cyclone* OR hurricane* OR *storm* OR "canopy gap*" OR rain* OR precipitation OR irrigat* OR disturb* OR “bark beetle*” OR pest OR “insect herbivore*” OR "insect infestation" OR "insect outbreak" OR "beetle outbreak" OR “pathogen*”) AND (biota OR fauna OR organism* OR micro?fauna OR macro?fauna OR meso?fauna OR animal* OR arthropod* OR invert* OR insect OR detritivore* OR macroarthropod* OR rotifer* OR mite* OR orbatid* OR acari* OR tardigrad* OR protist* OR micro-arthropod* OR microarthropod* OR ciliat* OR nematod* OR oligochaet* OR annelid*  OR enchytrae* OR potworm OR lumbricidae,  OR collembol* OR springtail* OR earthworm* OR enchytrae* OR lumbricid* OR “soil biodiversity” OR “below?ground biodiversity” OR “soil divers*” OR “below?ground divers*” OR biodiversity))</t>
   </si>
   <si>
@@ -167,6 +161,9 @@
   </si>
   <si>
     <t>Excluded full texts (no mean/median)</t>
+  </si>
+  <si>
+    <t>Excluded full texts (duplicated data)</t>
   </si>
 </sst>
 </file>
@@ -543,13 +540,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="195.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -560,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>9290</v>
@@ -574,7 +571,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>8275</v>
@@ -616,13 +613,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>9408</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="225" x14ac:dyDescent="0.25">
@@ -633,13 +630,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>9815</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="225" x14ac:dyDescent="0.25">
@@ -650,13 +647,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>9815</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -667,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>1649</v>
@@ -681,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>1191</v>
@@ -695,7 +692,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -713,10 +710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EC4C7B-DBA4-44D4-9484-D3F9181EAA9D}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +758,7 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1967</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -770,7 +767,7 @@
       </c>
       <c r="B6">
         <f>(B2+B3)-B5</f>
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,7 +775,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +784,7 @@
       </c>
       <c r="B8">
         <f>B5-B7</f>
-        <v>1885</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +792,7 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,7 +829,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -840,7 +837,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -848,111 +845,75 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <f>SUM(B13:B21,B10:B11)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
         <v>38</v>
       </c>
-      <c r="B21">
-        <f>SUM(B13:B20,B10:B11)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B22">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="e">
-        <f>#REF!-(#REF!+#REF!+#REF!+#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C32">
-        <f>121+49+315+19+27</f>
-        <v>531</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33">
-        <v>238</v>
-      </c>
-      <c r="C33">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>25</v>
+      <c r="B24">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>